<commit_message>
Changed baseline to initial, refactored method names
</commit_message>
<xml_diff>
--- a/nutrition/default_params.xlsx
+++ b/nutrition/default_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/nutrition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A673BBF9-766E-C141-81F0-6EE950CC20AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D33D9458-9EF1-DE4F-BA63-C8712241C8F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13020" yWindow="-21140" windowWidth="19200" windowHeight="21140" firstSheet="2" activeTab="3" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Programs impacted population" sheetId="14" r:id="rId1"/>
     <sheet name="Program risk areas" sheetId="15" r:id="rId2"/>
     <sheet name="Population risk areas" sheetId="16" r:id="rId3"/>
-    <sheet name="IYCF package odds ratios" sheetId="12" r:id="rId4"/>
+    <sheet name="IYCF odds ratios" sheetId="12" r:id="rId4"/>
     <sheet name="Appropriate breastfeeding" sheetId="13" r:id="rId5"/>
     <sheet name="Birth outcome risks" sheetId="2" r:id="rId6"/>
     <sheet name="Relative risks" sheetId="3" r:id="rId7"/>

</xml_diff>

<commit_message>
Setting the probability of birth outcome given spacing
</commit_message>
<xml_diff>
--- a/nutrition/default_params.xlsx
+++ b/nutrition/default_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/nutrition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BE7CD60D-B535-6D46-B36C-9C5E0FD327DE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{69A7711A-3B72-2640-A0F6-6950EC4E552B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs impacted population" sheetId="14" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Birth outcome risks'!$A$1:$F$7</definedName>
     <definedName name="abortion">'[1]Baseline year population inputs'!$C$26</definedName>
     <definedName name="food_insecure">'[1]Baseline year population inputs'!$C$3</definedName>
     <definedName name="frac_maize">'[1]Baseline year population inputs'!$C$14</definedName>
@@ -197,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="161">
   <si>
     <t>Neonatal other</t>
   </si>
@@ -812,7 +813,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -835,13 +836,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -948,6 +960,7 @@
     <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{126E324F-EC88-2347-908A-4D1058B147A7}"/>
@@ -1359,10 +1372,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2060,7 +2073,7 @@
       <c r="N16" s="46"/>
       <c r="O16" s="46"/>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43" t="s">
         <v>107</v>
       </c>
@@ -2107,7 +2120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43"/>
       <c r="B18" s="54" t="s">
         <v>102</v>
@@ -2152,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="34" t="s">
         <v>149</v>
       </c>
@@ -2196,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="34" t="s">
         <v>154</v>
       </c>
@@ -2240,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="55" t="s">
         <v>71</v>
       </c>
@@ -2284,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="54" t="s">
         <v>100</v>
       </c>
@@ -2328,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="54" t="s">
         <v>101</v>
       </c>
@@ -2372,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="54" t="s">
         <v>72</v>
       </c>
@@ -2416,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="54"/>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
@@ -2432,7 +2445,7 @@
       <c r="N25" s="46"/>
       <c r="O25" s="46"/>
     </row>
-    <row r="26" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
         <v>112</v>
       </c>
@@ -2470,16 +2483,17 @@
         <v>1</v>
       </c>
       <c r="M26" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="58"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="35" t="s">
         <v>150</v>
       </c>
@@ -2523,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43"/>
       <c r="B28" s="35" t="s">
         <v>151</v>
@@ -2568,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
         <v>152</v>
       </c>
@@ -2612,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
         <v>153</v>
       </c>
@@ -2656,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="54"/>
       <c r="C31" s="45"/>
       <c r="D31" s="45"/>
@@ -2672,7 +2686,7 @@
       <c r="N31" s="46"/>
       <c r="O31" s="46"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
         <v>111</v>
       </c>
@@ -5284,7 +5298,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5601,9 +5615,7 @@
       <c r="G12" s="50"/>
       <c r="H12" s="50"/>
       <c r="I12" s="50"/>
-      <c r="J12" s="50" t="s">
-        <v>118</v>
-      </c>
+      <c r="J12" s="50"/>
       <c r="K12" s="50" t="s">
         <v>118</v>
       </c>
@@ -5622,9 +5634,7 @@
       <c r="G13" s="50"/>
       <c r="H13" s="50"/>
       <c r="I13" s="50"/>
-      <c r="J13" s="50" t="s">
-        <v>118</v>
-      </c>
+      <c r="J13" s="50"/>
       <c r="K13" s="50" t="s">
         <v>118</v>
       </c>
@@ -5643,9 +5653,7 @@
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
       <c r="I14" s="50"/>
-      <c r="J14" s="50" t="s">
-        <v>118</v>
-      </c>
+      <c r="J14" s="50"/>
       <c r="K14" s="50" t="s">
         <v>118</v>
       </c>
@@ -6787,7 +6795,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10085,7 +10093,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10387,7 +10395,7 @@
         <v>119</v>
       </c>
       <c r="C21" s="57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="57">
         <v>1</v>

</xml_diff>

<commit_message>
Updated OR for optimal birth spacing
</commit_message>
<xml_diff>
--- a/nutrition/default_params.xlsx
+++ b/nutrition/default_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/nutrition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{69A7711A-3B72-2640-A0F6-6950EC4E552B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D1B4ACD3-D4B4-A945-A0EB-397DCF092165}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
   </bookViews>
@@ -674,13 +674,13 @@
     <t>Relative risk by birth spacing</t>
   </si>
   <si>
-    <t>Odds ratios for correct birth spacing by program</t>
-  </si>
-  <si>
     <t>Birth spacing</t>
   </si>
   <si>
     <t>Birth number</t>
+  </si>
+  <si>
+    <t>Odds ratios for optimal birth spacing by program</t>
   </si>
 </sst>
 </file>
@@ -853,7 +853,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -956,9 +956,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -2491,7 +2488,7 @@
       <c r="O26" s="50">
         <v>0</v>
       </c>
-      <c r="P26" s="58"/>
+      <c r="P26" s="57"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="35" t="s">
@@ -4597,10 +4594,10 @@
         <v>120</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -5298,7 +5295,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5345,10 +5342,10 @@
         <v>120</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -10093,7 +10090,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10373,7 +10370,7 @@
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -10394,16 +10391,16 @@
       <c r="B21" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="57">
-        <v>2</v>
-      </c>
-      <c r="D21" s="57">
-        <v>1</v>
-      </c>
-      <c r="E21" s="57">
-        <v>1</v>
-      </c>
-      <c r="F21" s="57">
+      <c r="C21" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed profilactic zinc supplementation
</commit_message>
<xml_diff>
--- a/nutrition/default_params.xlsx
+++ b/nutrition/default_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/nutrition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D1B4ACD3-D4B4-A945-A0EB-397DCF092165}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ECB35F06-6614-9940-96BE-9AB11F147AAC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
+    <workbookView xWindow="-140" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="10" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs impacted population" sheetId="14" r:id="rId1"/>
@@ -99,35 +99,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Janka Petravic</author>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LiST: 1.11</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000004000000}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000004000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000005000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000005000000}">
       <text>
         <r>
           <rPr>
@@ -198,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="160">
   <si>
     <t>Neonatal other</t>
   </si>
@@ -387,9 +362,6 @@
   </si>
   <si>
     <t>Public provision of complementary foods</t>
-  </si>
-  <si>
-    <t>Prophylactic zinc supplementation</t>
   </si>
   <si>
     <t>By program</t>
@@ -691,7 +663,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -732,19 +704,6 @@
     <font>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -937,15 +896,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -954,10 +913,10 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{126E324F-EC88-2347-908A-4D1058B147A7}"/>
@@ -1372,7 +1331,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1390,10 +1349,10 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="43" t="s">
         <v>36</v>
@@ -1437,10 +1396,10 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="50">
         <v>0</v>
@@ -1484,7 +1443,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="50">
         <v>1</v>
@@ -1528,7 +1487,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="50">
         <v>1</v>
@@ -1572,7 +1531,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="50">
         <v>1</v>
@@ -1616,7 +1575,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="50">
         <v>1</v>
@@ -1660,7 +1619,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="50">
         <v>1</v>
@@ -1748,7 +1707,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="50">
         <v>0</v>
@@ -1792,7 +1751,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="50">
         <v>1</v>
@@ -1880,7 +1839,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="50">
         <v>0</v>
@@ -1924,7 +1883,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="50">
         <v>0</v>
@@ -1968,7 +1927,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="50">
         <v>1</v>
@@ -2012,7 +1971,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="50">
         <v>0</v>
@@ -2072,10 +2031,10 @@
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="50">
         <v>0</v>
@@ -2120,7 +2079,7 @@
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43"/>
       <c r="B18" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="50">
         <v>0</v>
@@ -2164,7 +2123,7 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="50">
         <v>0</v>
@@ -2208,7 +2167,7 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C20" s="50">
         <v>0</v>
@@ -2252,7 +2211,7 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="50">
         <v>0</v>
@@ -2296,7 +2255,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="50">
         <v>0</v>
@@ -2340,7 +2299,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="50">
         <v>0</v>
@@ -2384,7 +2343,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="50">
         <v>0</v>
@@ -2444,10 +2403,10 @@
     </row>
     <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="50">
         <v>0</v>
@@ -2488,11 +2447,11 @@
       <c r="O26" s="50">
         <v>0</v>
       </c>
-      <c r="P26" s="57"/>
+      <c r="P26" s="56"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="50">
         <v>0</v>
@@ -2537,7 +2496,7 @@
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43"/>
       <c r="B28" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C28" s="50">
         <v>0</v>
@@ -2581,7 +2540,7 @@
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="50">
         <v>0</v>
@@ -2625,7 +2584,7 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30" s="50">
         <v>0</v>
@@ -2685,10 +2644,10 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" s="50">
         <v>1</v>
@@ -2732,7 +2691,7 @@
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33" s="50">
         <v>1</v>
@@ -2776,7 +2735,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" s="50">
         <v>1</v>
@@ -2820,7 +2779,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" s="50">
         <v>1</v>
@@ -2864,7 +2823,7 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="50">
         <v>1</v>
@@ -2909,7 +2868,7 @@
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="42"/>
       <c r="B37" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="50">
         <v>1</v>
@@ -2953,7 +2912,7 @@
     </row>
     <row r="38" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="50">
         <v>1</v>
@@ -2997,7 +2956,7 @@
     </row>
     <row r="39" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="50">
         <v>1</v>
@@ -3041,7 +3000,7 @@
     </row>
     <row r="40" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" s="50">
         <v>1</v>
@@ -3085,7 +3044,7 @@
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="50">
         <v>1</v>
@@ -3175,12 +3134,12 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -3200,7 +3159,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="36"/>
@@ -3211,7 +3170,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -3242,8 +3201,8 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3261,13 +3220,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>36</v>
@@ -3287,13 +3246,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -3313,7 +3272,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C3" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -3333,7 +3292,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C4" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -3359,7 +3318,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -3379,7 +3338,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C6" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -3402,7 +3361,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -3422,7 +3381,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C8" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -3448,7 +3407,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -3468,7 +3427,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C10" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -3491,7 +3450,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
@@ -3511,7 +3470,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C12" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -3531,13 +3490,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="54" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -3557,7 +3516,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C14" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -3581,7 +3540,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
@@ -3602,7 +3561,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C16" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="4">
         <v>0</v>
@@ -3623,13 +3582,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="4">
         <v>0.7</v>
@@ -3650,7 +3609,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C18" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" s="4">
         <v>0.46</v>
@@ -3671,13 +3630,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" s="4">
         <v>0.7</v>
@@ -3697,7 +3656,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" s="4">
         <v>0.46</v>
@@ -3717,13 +3676,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" s="4">
         <v>0.7</v>
@@ -3743,7 +3702,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C22" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="4">
         <v>0.46</v>
@@ -3763,13 +3722,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -3789,7 +3748,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C24" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D24" s="4">
         <v>0.17</v>
@@ -3809,7 +3768,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C25" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="4">
         <v>0.17</v>
@@ -3829,13 +3788,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -3855,7 +3814,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D27" s="4">
         <v>0.69</v>
@@ -3875,7 +3834,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C28" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="4">
         <v>0.69</v>
@@ -3895,13 +3854,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
@@ -3921,7 +3880,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30" s="4">
         <v>0.36</v>
@@ -3941,7 +3900,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D31" s="4">
         <v>0.36</v>
@@ -3961,13 +3920,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
@@ -3987,7 +3946,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C33" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D33" s="4">
         <v>0.2</v>
@@ -4007,7 +3966,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C34" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" s="4">
         <v>0.2</v>
@@ -4027,13 +3986,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
@@ -4053,7 +4012,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C36" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" s="4">
         <v>0.48</v>
@@ -4073,7 +4032,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C37" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D37" s="4">
         <v>0.48</v>
@@ -4093,13 +4052,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38" s="4">
         <v>0.3</v>
@@ -4119,7 +4078,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C39" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="4">
         <v>0.5</v>
@@ -4139,7 +4098,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C40" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" s="4">
         <v>0.65</v>
@@ -4162,7 +4121,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41" s="4">
         <v>0.3</v>
@@ -4182,7 +4141,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C42" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" s="4">
         <v>0.49</v>
@@ -4202,7 +4161,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C43" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" s="4">
         <v>0.52</v>
@@ -4222,13 +4181,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" s="4">
         <v>0.88</v>
@@ -4248,7 +4207,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C45" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D45" s="4">
         <v>0.93</v>
@@ -4268,13 +4227,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="54" t="s">
         <v>41</v>
       </c>
       <c r="C46" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
@@ -4294,7 +4253,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C47" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D47" s="4">
         <v>0.86</v>
@@ -4314,13 +4273,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" s="54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B48" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D48" s="4">
         <v>0.57999999999999996</v>
@@ -4340,7 +4299,7 @@
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C49" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D49" s="4">
         <v>0.51</v>
@@ -4386,10 +4345,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="2" t="s">
@@ -4408,13 +4367,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -4432,7 +4391,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="4">
         <v>0.2</v>
@@ -4450,13 +4409,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -4475,7 +4434,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="27"/>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="4">
         <v>0.59</v>
@@ -4493,13 +4452,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -4518,7 +4477,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="27"/>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="4">
         <v>0.6</v>
@@ -4547,7 +4506,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4567,42 +4526,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -4612,14 +4571,14 @@
       <c r="G2" s="50"/>
       <c r="H2" s="50"/>
       <c r="I2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J2" s="50"/>
       <c r="K2" s="50"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -4628,7 +4587,7 @@
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
       <c r="H3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I3" s="50"/>
       <c r="J3" s="50"/>
@@ -4636,12 +4595,12 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
       <c r="D4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="50"/>
@@ -4653,11 +4612,11 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50"/>
@@ -4670,7 +4629,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -4681,26 +4640,26 @@
       <c r="H6" s="50"/>
       <c r="I6" s="50"/>
       <c r="J6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
       <c r="H7" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="50"/>
@@ -4708,18 +4667,18 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
       <c r="H8" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50"/>
@@ -4727,18 +4686,18 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
       <c r="H9" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="50"/>
@@ -4746,11 +4705,11 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
@@ -4763,11 +4722,11 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -4780,11 +4739,11 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -4797,11 +4756,11 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
@@ -4814,11 +4773,11 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -4826,18 +4785,18 @@
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
       <c r="I14" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="50"/>
@@ -4845,39 +4804,39 @@
       <c r="G15" s="50"/>
       <c r="H15" s="50"/>
       <c r="I15" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="50"/>
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
       <c r="G16" s="50"/>
       <c r="H16" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
@@ -4890,16 +4849,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
       <c r="F18" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G18" s="50"/>
       <c r="H18" s="50"/>
@@ -4909,16 +4868,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="50"/>
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
       <c r="F19" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G19" s="50"/>
       <c r="H19" s="50"/>
@@ -4928,16 +4887,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
       <c r="F20" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="50"/>
       <c r="H20" s="50"/>
@@ -4947,7 +4906,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
@@ -4956,10 +4915,10 @@
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
       <c r="H21" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I21" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
@@ -4969,13 +4928,13 @@
         <v>61</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
@@ -4987,11 +4946,11 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="50"/>
       <c r="C23" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
@@ -4999,14 +4958,14 @@
       <c r="G23" s="50"/>
       <c r="H23" s="50"/>
       <c r="I23" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J23" s="50"/>
       <c r="K23" s="50"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="50"/>
       <c r="C24" s="50"/>
@@ -5015,7 +4974,7 @@
       <c r="F24" s="50"/>
       <c r="G24" s="50"/>
       <c r="H24" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I24" s="50"/>
       <c r="J24" s="50"/>
@@ -5023,7 +4982,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
@@ -5032,7 +4991,7 @@
       <c r="F25" s="50"/>
       <c r="G25" s="50"/>
       <c r="H25" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I25" s="50"/>
       <c r="J25" s="50"/>
@@ -5040,11 +4999,11 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="50"/>
       <c r="C26" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
@@ -5057,11 +5016,11 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="50"/>
       <c r="C27" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
@@ -5069,14 +5028,14 @@
       <c r="G27" s="50"/>
       <c r="H27" s="50"/>
       <c r="I27" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J27" s="50"/>
       <c r="K27" s="50"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>
@@ -5085,7 +5044,7 @@
       <c r="F28" s="50"/>
       <c r="G28" s="50"/>
       <c r="H28" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I28" s="50"/>
       <c r="J28" s="50"/>
@@ -5096,11 +5055,11 @@
         <v>62</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29" s="50"/>
       <c r="D29" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
@@ -5112,13 +5071,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="50"/>
       <c r="C30" s="50"/>
       <c r="D30" s="50"/>
       <c r="E30" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F30" s="50"/>
       <c r="G30" s="50"/>
@@ -5129,7 +5088,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B31" s="50"/>
       <c r="C31" s="50"/>
@@ -5137,10 +5096,10 @@
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
       <c r="G31" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H31" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I31" s="50"/>
       <c r="J31" s="50"/>
@@ -5148,7 +5107,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="50"/>
       <c r="C32" s="50"/>
@@ -5156,10 +5115,10 @@
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
       <c r="G32" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H32" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I32" s="50"/>
       <c r="J32" s="50"/>
@@ -5167,7 +5126,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="50"/>
       <c r="C33" s="50"/>
@@ -5175,10 +5134,10 @@
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
       <c r="G33" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H33" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I33" s="50"/>
       <c r="J33" s="50"/>
@@ -5186,7 +5145,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A34" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" s="50"/>
       <c r="C34" s="50"/>
@@ -5194,10 +5153,10 @@
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
       <c r="G34" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H34" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I34" s="50"/>
       <c r="J34" s="50"/>
@@ -5205,7 +5164,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="50"/>
       <c r="C35" s="50"/>
@@ -5213,10 +5172,10 @@
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
       <c r="G35" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H35" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I35" s="50"/>
       <c r="J35" s="50"/>
@@ -5224,7 +5183,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A36" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" s="50"/>
       <c r="C36" s="50"/>
@@ -5232,10 +5191,10 @@
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
       <c r="G36" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H36" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I36" s="50"/>
       <c r="J36" s="50"/>
@@ -5243,7 +5202,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A37" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" s="50"/>
       <c r="C37" s="50"/>
@@ -5252,7 +5211,7 @@
       <c r="F37" s="50"/>
       <c r="G37" s="50"/>
       <c r="H37" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I37" s="50"/>
       <c r="J37" s="50"/>
@@ -5260,20 +5219,20 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A38" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38" s="50"/>
       <c r="D38" s="50"/>
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
       <c r="G38" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H38" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I38" s="50"/>
       <c r="J38" s="50"/>
@@ -5315,37 +5274,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -5353,25 +5312,25 @@
         <v>36</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I2" s="50"/>
       <c r="J2" s="50"/>
@@ -5382,25 +5341,25 @@
         <v>35</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H3" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I3" s="50"/>
       <c r="J3" s="50"/>
@@ -5411,25 +5370,25 @@
         <v>34</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I4" s="50"/>
       <c r="J4" s="50"/>
@@ -5440,25 +5399,25 @@
         <v>33</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I5" s="50"/>
       <c r="J5" s="50"/>
@@ -5469,25 +5428,25 @@
         <v>32</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I6" s="50"/>
       <c r="J6" s="50"/>
@@ -5499,17 +5458,17 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
       <c r="H7" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
@@ -5520,17 +5479,17 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
       <c r="H8" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I8" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
@@ -5541,17 +5500,17 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
       <c r="H9" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J9" s="50"/>
       <c r="K9" s="50"/>
@@ -5562,17 +5521,17 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
       <c r="H10" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I10" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
@@ -5583,7 +5542,7 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -5592,10 +5551,10 @@
       <c r="H11" s="50"/>
       <c r="I11" s="50"/>
       <c r="J11" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K11" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -5604,7 +5563,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -5614,7 +5573,7 @@
       <c r="I12" s="50"/>
       <c r="J12" s="50"/>
       <c r="K12" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
@@ -5623,7 +5582,7 @@
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
@@ -5633,7 +5592,7 @@
       <c r="I13" s="50"/>
       <c r="J13" s="50"/>
       <c r="K13" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -5642,7 +5601,7 @@
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -5652,7 +5611,7 @@
       <c r="I14" s="50"/>
       <c r="J14" s="50"/>
       <c r="K14" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -5681,13 +5640,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>36</v>
@@ -5707,13 +5666,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" s="56" t="s">
-        <v>107</v>
+        <v>133</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="49">
         <v>1</v>
@@ -5732,55 +5691,55 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="56"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="49">
+        <v>1</v>
+      </c>
+      <c r="E3" s="49">
+        <v>1</v>
+      </c>
+      <c r="F3" s="49">
+        <v>1</v>
+      </c>
+      <c r="G3" s="49">
+        <v>1</v>
+      </c>
+      <c r="H3" s="49">
+        <v>1</v>
+      </c>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B4" s="57"/>
+      <c r="C4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="49">
+        <v>1</v>
+      </c>
+      <c r="E4" s="49">
+        <v>1</v>
+      </c>
+      <c r="F4" s="49">
+        <v>1</v>
+      </c>
+      <c r="G4" s="49">
+        <v>1</v>
+      </c>
+      <c r="H4" s="49">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B5" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D3" s="49">
-        <v>1</v>
-      </c>
-      <c r="E3" s="49">
-        <v>1</v>
-      </c>
-      <c r="F3" s="49">
-        <v>1</v>
-      </c>
-      <c r="G3" s="49">
-        <v>1</v>
-      </c>
-      <c r="H3" s="49">
-        <v>1</v>
-      </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="56"/>
-      <c r="C4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="49">
-        <v>1</v>
-      </c>
-      <c r="E4" s="49">
-        <v>1</v>
-      </c>
-      <c r="F4" s="49">
-        <v>1</v>
-      </c>
-      <c r="G4" s="49">
-        <v>1</v>
-      </c>
-      <c r="H4" s="49">
-        <v>1</v>
-      </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="D5" s="49">
         <f>5.16</f>
@@ -5800,9 +5759,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="56"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="49">
         <v>5.16</v>
@@ -5821,9 +5780,9 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="49">
         <v>1</v>
@@ -5842,11 +5801,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="57" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="49">
         <v>1</v>
@@ -5865,9 +5824,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="49">
         <v>1</v>
@@ -5886,9 +5845,9 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="49">
         <v>1</v>
@@ -5907,11 +5866,11 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="57" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="49">
         <v>1</v>
@@ -5930,9 +5889,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="56"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" s="49">
         <v>1</v>
@@ -5951,9 +5910,9 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="49">
         <v>1</v>
@@ -5972,11 +5931,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="57" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" s="49">
         <v>1</v>
@@ -5995,9 +5954,9 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="49">
         <v>1</v>
@@ -6016,9 +5975,9 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D16" s="49">
         <v>1</v>
@@ -6038,10 +5997,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B17" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="48">
         <v>1.05</v>
@@ -6061,13 +6020,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" s="56" t="s">
-        <v>107</v>
+        <v>135</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="49">
         <v>1</v>
@@ -6086,9 +6045,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" s="49">
         <v>1</v>
@@ -6107,9 +6066,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="56"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" s="49">
         <v>1</v>
@@ -6128,11 +6087,11 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="57" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" s="49">
         <v>1</v>
@@ -6151,9 +6110,9 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="56"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="49">
         <v>1</v>
@@ -6172,9 +6131,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="56"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="49">
         <v>1</v>
@@ -6193,11 +6152,11 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="57" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="49">
         <v>1</v>
@@ -6216,9 +6175,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="56"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" s="49">
         <v>1</v>
@@ -6237,9 +6196,9 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="56"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="49">
         <v>1</v>
@@ -6258,11 +6217,11 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="57" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="49">
         <v>1</v>
@@ -6281,9 +6240,9 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="56"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="49">
         <v>1</v>
@@ -6302,9 +6261,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="56"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" s="49">
         <v>1</v>
@@ -6323,11 +6282,11 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="57" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D31" s="49">
         <v>1</v>
@@ -6346,9 +6305,9 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="56"/>
+      <c r="B32" s="57"/>
       <c r="C32" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" s="49">
         <v>1</v>
@@ -6367,9 +6326,9 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="56"/>
+      <c r="B33" s="57"/>
       <c r="C33" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" s="49">
         <v>1</v>
@@ -6389,10 +6348,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B34" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D34" s="48">
         <v>1</v>
@@ -6412,13 +6371,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="B36" s="56" t="s">
-        <v>107</v>
+        <v>134</v>
+      </c>
+      <c r="B36" s="57" t="s">
+        <v>106</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="49">
         <v>1</v>
@@ -6437,54 +6396,54 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B37" s="56"/>
+      <c r="B37" s="57"/>
       <c r="C37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="49">
+        <v>1</v>
+      </c>
+      <c r="E37" s="49">
+        <v>1</v>
+      </c>
+      <c r="F37" s="49">
+        <v>1</v>
+      </c>
+      <c r="G37" s="49">
+        <v>1</v>
+      </c>
+      <c r="H37" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B38" s="57"/>
+      <c r="C38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="49">
+        <v>1</v>
+      </c>
+      <c r="E38" s="49">
+        <v>1</v>
+      </c>
+      <c r="F38" s="49">
+        <v>1</v>
+      </c>
+      <c r="G38" s="49">
+        <v>1</v>
+      </c>
+      <c r="H38" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B39" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="49">
-        <v>1</v>
-      </c>
-      <c r="E37" s="49">
-        <v>1</v>
-      </c>
-      <c r="F37" s="49">
-        <v>1</v>
-      </c>
-      <c r="G37" s="49">
-        <v>1</v>
-      </c>
-      <c r="H37" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B38" s="56"/>
-      <c r="C38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D38" s="49">
-        <v>1</v>
-      </c>
-      <c r="E38" s="49">
-        <v>1</v>
-      </c>
-      <c r="F38" s="49">
-        <v>1</v>
-      </c>
-      <c r="G38" s="49">
-        <v>1</v>
-      </c>
-      <c r="H38" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B39" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="D39" s="49">
         <v>1</v>
       </c>
@@ -6502,54 +6461,54 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B40" s="56"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="49">
+        <v>1</v>
+      </c>
+      <c r="E40" s="49">
+        <v>1</v>
+      </c>
+      <c r="F40" s="49">
+        <v>1</v>
+      </c>
+      <c r="G40" s="49">
+        <v>1</v>
+      </c>
+      <c r="H40" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B41" s="57"/>
+      <c r="C41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="49">
+        <v>1</v>
+      </c>
+      <c r="E41" s="49">
+        <v>1</v>
+      </c>
+      <c r="F41" s="49">
+        <v>1</v>
+      </c>
+      <c r="G41" s="49">
+        <v>1</v>
+      </c>
+      <c r="H41" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B42" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="49">
-        <v>1</v>
-      </c>
-      <c r="E40" s="49">
-        <v>1</v>
-      </c>
-      <c r="F40" s="49">
-        <v>1</v>
-      </c>
-      <c r="G40" s="49">
-        <v>1</v>
-      </c>
-      <c r="H40" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B41" s="56"/>
-      <c r="C41" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="49">
-        <v>1</v>
-      </c>
-      <c r="E41" s="49">
-        <v>1</v>
-      </c>
-      <c r="F41" s="49">
-        <v>1</v>
-      </c>
-      <c r="G41" s="49">
-        <v>1</v>
-      </c>
-      <c r="H41" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="D42" s="49">
         <v>1</v>
       </c>
@@ -6567,53 +6526,53 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B43" s="56"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="49">
+        <v>1</v>
+      </c>
+      <c r="E43" s="49">
+        <v>1</v>
+      </c>
+      <c r="F43" s="49">
+        <v>1</v>
+      </c>
+      <c r="G43" s="49">
+        <v>1</v>
+      </c>
+      <c r="H43" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B44" s="57"/>
+      <c r="C44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="49">
+        <v>1</v>
+      </c>
+      <c r="E44" s="49">
+        <v>1</v>
+      </c>
+      <c r="F44" s="49">
+        <v>1</v>
+      </c>
+      <c r="G44" s="49">
+        <v>1</v>
+      </c>
+      <c r="H44" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B45" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D43" s="49">
-        <v>1</v>
-      </c>
-      <c r="E43" s="49">
-        <v>1</v>
-      </c>
-      <c r="F43" s="49">
-        <v>1</v>
-      </c>
-      <c r="G43" s="49">
-        <v>1</v>
-      </c>
-      <c r="H43" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B44" s="56"/>
-      <c r="C44" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="49">
-        <v>1</v>
-      </c>
-      <c r="E44" s="49">
-        <v>1</v>
-      </c>
-      <c r="F44" s="49">
-        <v>1</v>
-      </c>
-      <c r="G44" s="49">
-        <v>1</v>
-      </c>
-      <c r="H44" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B45" s="56" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="D45" s="49">
         <v>1</v>
@@ -6632,9 +6591,9 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B46" s="56"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" s="49">
         <v>1</v>
@@ -6653,9 +6612,9 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B47" s="56"/>
+      <c r="B47" s="57"/>
       <c r="C47" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D47" s="49">
         <v>1</v>
@@ -6674,11 +6633,11 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="57" t="s">
         <v>33</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D48" s="49">
         <v>1</v>
@@ -6697,9 +6656,9 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="56"/>
+      <c r="B49" s="57"/>
       <c r="C49" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D49" s="49">
         <v>1</v>
@@ -6718,9 +6677,9 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="56"/>
+      <c r="B50" s="57"/>
       <c r="C50" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D50" s="49">
         <v>1</v>
@@ -6740,10 +6699,10 @@
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B51" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D51" s="48">
         <v>1.05</v>
@@ -6763,6 +6722,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -6773,11 +6737,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6827,7 +6786,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="21"/>
@@ -7209,7 +7168,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>42</v>
@@ -7247,7 +7206,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -7275,7 +7234,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C4" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -7303,7 +7262,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C5" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -7331,7 +7290,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C6" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -7362,7 +7321,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
@@ -7390,7 +7349,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C8" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -7418,7 +7377,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C9" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -7446,7 +7405,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C10" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -7477,7 +7436,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -7505,7 +7464,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C12" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -7533,7 +7492,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C13" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -7561,7 +7520,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C14" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -7592,7 +7551,7 @@
         <v>48</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -7620,7 +7579,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C16" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -7648,7 +7607,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C17" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -7676,7 +7635,7 @@
     </row>
     <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C18" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -7707,7 +7666,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
@@ -7735,7 +7694,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C20" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -7763,7 +7722,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C21" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -7791,7 +7750,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C22" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -7822,7 +7781,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
@@ -7850,7 +7809,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C24" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -7878,7 +7837,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C25" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
@@ -7906,7 +7865,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C26" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -7939,7 +7898,7 @@
     </row>
     <row r="29" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>42</v>
@@ -7977,7 +7936,7 @@
         <v>41</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D30" s="5">
         <v>1</v>
@@ -8005,7 +7964,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C31" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
@@ -8092,7 +8051,7 @@
         <v>40</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D34" s="5">
         <v>1</v>
@@ -8120,7 +8079,7 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C35" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
@@ -8207,7 +8166,7 @@
         <v>49</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D38" s="5">
         <v>1</v>
@@ -8235,7 +8194,7 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C39" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
@@ -8322,7 +8281,7 @@
         <v>48</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D42" s="5">
         <v>1</v>
@@ -8350,7 +8309,7 @@
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C43" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -8437,7 +8396,7 @@
         <v>39</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D46" s="5">
         <v>1</v>
@@ -8465,7 +8424,7 @@
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C47" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -8552,7 +8511,7 @@
         <v>47</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D50" s="5">
         <v>1</v>
@@ -8580,7 +8539,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C51" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D51" s="4">
         <v>1</v>
@@ -8673,7 +8632,7 @@
     </row>
     <row r="56" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A56" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" s="30" t="s">
         <v>42</v>
@@ -8705,7 +8664,7 @@
         <v>46</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" s="5">
         <v>1</v>
@@ -8727,7 +8686,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C58" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D58" s="4">
         <v>10.675000000000001</v>
@@ -8752,7 +8711,7 @@
         <v>45</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
@@ -8774,7 +8733,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C60" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D60" s="4">
         <v>10.675000000000001</v>
@@ -8799,7 +8758,7 @@
         <v>44</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
@@ -8821,7 +8780,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C62" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D62" s="4">
         <v>10.675000000000001</v>
@@ -8852,7 +8811,7 @@
     </row>
     <row r="65" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A65" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B65" s="30" t="s">
         <v>42</v>
@@ -8890,7 +8849,7 @@
         <v>7</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D66" s="5">
         <v>1</v>
@@ -8918,7 +8877,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C67" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D67" s="4">
         <v>1.35</v>
@@ -8946,7 +8905,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C68" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D68" s="4">
         <v>1.35</v>
@@ -8974,7 +8933,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C69" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D69" s="4">
         <v>5.4</v>
@@ -9005,7 +8964,7 @@
         <v>6</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D70" s="5">
         <v>1</v>
@@ -9033,7 +8992,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C71" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D71" s="4">
         <v>1.35</v>
@@ -9061,7 +9020,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C72" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D72" s="4">
         <v>1.35</v>
@@ -9089,7 +9048,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C73" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D73" s="4">
         <v>5.4</v>
@@ -9120,7 +9079,7 @@
         <v>5</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D74" s="5">
         <v>1</v>
@@ -9148,7 +9107,7 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C75" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D75" s="4">
         <v>1.35</v>
@@ -9176,7 +9135,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C76" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D76" s="4">
         <v>1.35</v>
@@ -9204,7 +9163,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C77" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D77" s="4">
         <v>5.4</v>
@@ -9235,7 +9194,7 @@
         <v>3</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D78" s="5">
         <v>1</v>
@@ -9263,7 +9222,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C79" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D79" s="4">
         <v>1</v>
@@ -9291,7 +9250,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C80" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -9319,7 +9278,7 @@
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C81" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D81" s="4">
         <v>1</v>
@@ -9350,7 +9309,7 @@
         <v>41</v>
       </c>
       <c r="C82" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D82" s="5">
         <v>1</v>
@@ -9378,7 +9337,7 @@
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C83" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D83" s="4">
         <v>1</v>
@@ -9406,7 +9365,7 @@
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C84" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D84" s="4">
         <v>1</v>
@@ -9434,7 +9393,7 @@
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C85" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D85" s="4">
         <v>1</v>
@@ -9465,7 +9424,7 @@
         <v>40</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D86" s="5">
         <v>1</v>
@@ -9493,7 +9452,7 @@
     </row>
     <row r="87" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C87" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D87" s="4">
         <v>1</v>
@@ -9521,7 +9480,7 @@
     </row>
     <row r="88" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C88" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D88" s="4">
         <v>1</v>
@@ -9549,7 +9508,7 @@
     </row>
     <row r="89" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C89" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D89" s="4">
         <v>1</v>
@@ -9580,7 +9539,7 @@
         <v>49</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D90" s="5">
         <v>1</v>
@@ -9608,7 +9567,7 @@
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C91" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D91" s="4">
         <v>1</v>
@@ -9636,7 +9595,7 @@
     </row>
     <row r="92" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C92" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D92" s="4">
         <v>1</v>
@@ -9664,7 +9623,7 @@
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C93" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D93" s="4">
         <v>1</v>
@@ -9695,7 +9654,7 @@
         <v>39</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D94" s="5">
         <v>1</v>
@@ -9723,7 +9682,7 @@
     </row>
     <row r="95" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C95" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D95" s="4">
         <v>1</v>
@@ -9751,7 +9710,7 @@
     </row>
     <row r="96" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C96" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D96" s="4">
         <v>1</v>
@@ -9779,7 +9738,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C97" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D97" s="4">
         <v>1</v>
@@ -9807,10 +9766,10 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B98" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D98" s="5">
         <v>1</v>
@@ -9838,7 +9797,7 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C99" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D99" s="4">
         <v>1</v>
@@ -9866,7 +9825,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C100" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D100" s="4">
         <v>1</v>
@@ -9894,7 +9853,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C101" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D101" s="4">
         <v>1</v>
@@ -9930,7 +9889,7 @@
         <v>41</v>
       </c>
       <c r="B104" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C104" s="29" t="s">
         <v>37</v>
@@ -9963,7 +9922,7 @@
       <c r="A105" s="2"/>
       <c r="B105" s="27"/>
       <c r="C105" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D105" s="5">
         <v>1</v>
@@ -9991,7 +9950,7 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C106" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D106" s="4">
         <v>1.26</v>
@@ -10019,7 +9978,7 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C107" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D107" s="4">
         <v>1.68</v>
@@ -10047,7 +10006,7 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C108" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D108" s="4">
         <v>2.65</v>
@@ -10087,10 +10046,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10107,12 +10066,12 @@
   <sheetData>
     <row r="1" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="2" t="s">
@@ -10133,10 +10092,10 @@
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="4">
         <v>45</v>
@@ -10154,7 +10113,7 @@
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="4">
         <v>1.0249999999999999</v>
@@ -10174,12 +10133,12 @@
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -10188,18 +10147,18 @@
         <v>1</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="F6" s="4">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="G6" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -10219,7 +10178,7 @@
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="6" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -10228,84 +10187,85 @@
         <v>1</v>
       </c>
       <c r="E8" s="4">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="18" t="s">
-        <v>156</v>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="10"/>
+      <c r="B11" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.39</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
-      <c r="B12" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.39</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10"/>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="18" t="s">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="18" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="51" t="s">
-        <v>131</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="4">
         <v>1.0249999999999999</v>
@@ -10324,9 +10284,11 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2"/>
-      <c r="B16" s="6" t="s">
-        <v>58</v>
+      <c r="A16" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C16" s="4">
         <v>1.0249999999999999</v>
@@ -10344,63 +10306,40 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1.0249999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C20" s="43" t="s">
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="1:6" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C19" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D19" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="43" t="s">
+      <c r="F19" s="43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B21" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="4">
         <v>1.52</v>
       </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4">
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
         <v>1</v>
       </c>
     </row>
@@ -10433,7 +10372,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
@@ -10451,10 +10390,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4">
         <v>0.21</v>
@@ -10472,7 +10411,7 @@
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="34"/>
       <c r="B3" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -10489,10 +10428,10 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4">
         <v>0.15</v>
@@ -10510,7 +10449,7 @@
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="34"/>
       <c r="B5" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -10527,10 +10466,10 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="4">
         <v>0.15</v>
@@ -10548,7 +10487,7 @@
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="34"/>
       <c r="B7" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -10565,10 +10504,10 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4">
         <v>0.35</v>
@@ -10586,7 +10525,7 @@
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="34"/>
       <c r="B9" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -10603,10 +10542,10 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="4">
         <v>0.35</v>
@@ -10624,7 +10563,7 @@
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="34"/>
       <c r="B11" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -10641,10 +10580,10 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="4">
         <v>0.23</v>
@@ -10662,7 +10601,7 @@
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="34"/>
       <c r="B13" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -10753,12 +10692,12 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="4">
         <v>0.53</v>
@@ -10802,7 +10741,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B4" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
@@ -10846,7 +10785,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -10890,7 +10829,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -10934,7 +10873,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -10978,7 +10917,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B8" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -11022,7 +10961,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -11066,7 +11005,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B10" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -11154,7 +11093,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B12" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="4">
         <v>0.83</v>
@@ -11198,7 +11137,7 @@
     </row>
     <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -11242,7 +11181,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B14" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -11286,13 +11225,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="35"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B17" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -11336,7 +11275,7 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B18" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -11380,7 +11319,7 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B19" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
@@ -11424,7 +11363,7 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B20" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Changed impact of wash on diarrhoea incidence and mortality to 0
</commit_message>
<xml_diff>
--- a/nutrition/default_params.xlsx
+++ b/nutrition/default_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/nutrition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ECB35F06-6614-9940-96BE-9AB11F147AAC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ADD698E6-F3DA-8746-AD64-56E48666EE7D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="10" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="10" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Programs impacted population" sheetId="14" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <definedName name="stillbirth">'[1]Baseline year population inputs'!$C$27</definedName>
     <definedName name="term_SGA">'[1]Baseline year population inputs'!$C$35</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913" calcMode="manual" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3202,7 +3202,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3751,19 +3751,19 @@
         <v>84</v>
       </c>
       <c r="D24" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="E24" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="G24" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="H24" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
@@ -3771,19 +3771,19 @@
         <v>88</v>
       </c>
       <c r="D25" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="E25" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="G25" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="H25" s="4">
-        <v>0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
@@ -3817,19 +3817,19 @@
         <v>84</v>
       </c>
       <c r="D27" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="E27" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="H27" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
@@ -3837,19 +3837,19 @@
         <v>88</v>
       </c>
       <c r="D28" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="E28" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="F28" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="G28" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="H28" s="4">
-        <v>0.69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
@@ -3883,19 +3883,19 @@
         <v>84</v>
       </c>
       <c r="D30" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="E30" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="F30" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="G30" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="H30" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
@@ -3903,19 +3903,19 @@
         <v>88</v>
       </c>
       <c r="D31" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="E31" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="G31" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="H31" s="4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
@@ -3949,19 +3949,19 @@
         <v>84</v>
       </c>
       <c r="D33" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E33" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G33" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H33" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
@@ -3969,19 +3969,19 @@
         <v>88</v>
       </c>
       <c r="D34" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E34" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G34" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H34" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
@@ -4015,19 +4015,19 @@
         <v>84</v>
       </c>
       <c r="D36" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="E36" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="F36" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="G36" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="H36" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
@@ -4035,19 +4035,19 @@
         <v>88</v>
       </c>
       <c r="D37" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="E37" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="F37" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="G37" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="H37" s="4">
-        <v>0.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
@@ -6722,6 +6722,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -6731,11 +6736,6 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B36:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Turn off link between diarrhoea and anaemia
</commit_message>
<xml_diff>
--- a/nutrition/default_params.xlsx
+++ b/nutrition/default_params.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/nutrition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{37DA4D6A-A558-744C-A270-76FCBBC9C600}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="10" xr2:uid="{9D310A7F-FF26-7448-8337-E29F42B35A9E}"/>
+    <workbookView xWindow="-38400" yWindow="-21144" windowWidth="38400" windowHeight="21144" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Programs impacted population" sheetId="14" r:id="rId1"/>
@@ -54,12 +53,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
+    <comment ref="A36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,12 +96,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000004000000}">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000005000000}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -658,10 +657,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -810,7 +809,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -879,7 +878,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -919,9 +918,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma 2" xfId="2" xr:uid="{126E324F-EC88-2347-908A-4D1058B147A7}"/>
+    <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{BB5D12A2-9228-9D4C-A4D1-BB58F8453394}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -941,88 +940,9 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Baseline year population inputs"/>
-      <sheetName val="Causes of death"/>
-      <sheetName val="Demographic projections"/>
-      <sheetName val="Nutritional status distribution"/>
-      <sheetName val="Breastfeeding distribution"/>
-      <sheetName val="Time trends"/>
-      <sheetName val="Fertility risks"/>
-      <sheetName val="Incidence of conditions"/>
-      <sheetName val="Programs target population"/>
-      <sheetName val="Programs family planning"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="C3">
-            <v>0.36</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>0.35199999999999998</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>0.8</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>0.12</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>0.05</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>34.68</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>39.32</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>3.1E-2</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>0.109</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>0.36499999999999999</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>0.42</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1324,7 +1244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72500D8E-E1F8-2749-A3FA-E0EDE33D10C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1334,20 +1254,20 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.83203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.1640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.796875" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.796875" style="41" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.19921875" style="41" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="14.5" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>116</v>
       </c>
@@ -1394,7 +1314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>115</v>
       </c>
@@ -1441,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="54" t="s">
         <v>127</v>
       </c>
@@ -1485,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="54" t="s">
         <v>114</v>
       </c>
@@ -1529,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="54" t="s">
         <v>113</v>
       </c>
@@ -1573,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="54" t="s">
         <v>112</v>
       </c>
@@ -1617,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="54" t="s">
         <v>154</v>
       </c>
@@ -1661,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="54" t="s">
         <v>61</v>
       </c>
@@ -1705,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="54" t="s">
         <v>79</v>
       </c>
@@ -1749,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="54" t="s">
         <v>87</v>
       </c>
@@ -1793,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="54" t="s">
         <v>62</v>
       </c>
@@ -1837,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="54" t="s">
         <v>82</v>
       </c>
@@ -1881,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="54" t="s">
         <v>96</v>
       </c>
@@ -1925,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="54" t="s">
         <v>86</v>
       </c>
@@ -1969,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="54" t="s">
         <v>89</v>
       </c>
@@ -2013,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="54"/>
       <c r="C16" s="46"/>
       <c r="D16" s="46"/>
@@ -2029,7 +1949,7 @@
       <c r="N16" s="46"/>
       <c r="O16" s="46"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
         <v>106</v>
       </c>
@@ -2076,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="43"/>
       <c r="B18" s="54" t="s">
         <v>101</v>
@@ -2121,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="34" t="s">
         <v>148</v>
       </c>
@@ -2165,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="34" t="s">
         <v>153</v>
       </c>
@@ -2209,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="55" t="s">
         <v>70</v>
       </c>
@@ -2253,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="54" t="s">
         <v>99</v>
       </c>
@@ -2297,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="54" t="s">
         <v>100</v>
       </c>
@@ -2341,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="54" t="s">
         <v>71</v>
       </c>
@@ -2385,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="54"/>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
@@ -2401,7 +2321,7 @@
       <c r="N25" s="46"/>
       <c r="O25" s="46"/>
     </row>
-    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="43" t="s">
         <v>111</v>
       </c>
@@ -2449,7 +2369,7 @@
       </c>
       <c r="P26" s="56"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="35" t="s">
         <v>149</v>
       </c>
@@ -2493,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
       <c r="B28" s="35" t="s">
         <v>150</v>
@@ -2538,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="35" t="s">
         <v>151</v>
       </c>
@@ -2582,7 +2502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="35" t="s">
         <v>152</v>
       </c>
@@ -2626,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="54"/>
       <c r="C31" s="45"/>
       <c r="D31" s="45"/>
@@ -2642,7 +2562,7 @@
       <c r="N31" s="46"/>
       <c r="O31" s="46"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="43" t="s">
         <v>110</v>
       </c>
@@ -2689,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="54" t="s">
         <v>74</v>
       </c>
@@ -2733,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="54" t="s">
         <v>76</v>
       </c>
@@ -2777,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="54" t="s">
         <v>77</v>
       </c>
@@ -2821,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="54" t="s">
         <v>69</v>
       </c>
@@ -2865,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="42"/>
       <c r="B37" s="54" t="s">
         <v>90</v>
@@ -2910,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="54" t="s">
         <v>91</v>
       </c>
@@ -2954,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="54" t="s">
         <v>92</v>
       </c>
@@ -2998,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="54" t="s">
         <v>94</v>
       </c>
@@ -3042,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="54" t="s">
         <v>93</v>
       </c>
@@ -3095,7 +3015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA57883-F6BA-144A-B403-BD5A394A6420}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3105,15 +3025,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.19921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
     <col min="3" max="7" width="14" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="33"/>
       <c r="C1" s="2" t="s">
@@ -3132,12 +3052,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="35" t="s">
         <v>82</v>
       </c>
@@ -3157,7 +3077,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -3168,7 +3088,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>147</v>
       </c>
@@ -3195,30 +3115,30 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9040D3C6-3BDE-7241-8EB1-F5AB6DDCE405}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" style="54" customWidth="1"/>
+    <col min="1" max="1" width="47.69921875" style="54" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="54" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="54" customWidth="1"/>
+    <col min="3" max="3" width="22.296875" style="54" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="1"/>
-    <col min="8" max="8" width="15.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -3244,7 +3164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>96</v>
       </c>
@@ -3270,7 +3190,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="54" t="s">
         <v>84</v>
       </c>
@@ -3290,7 +3210,7 @@
         <v>0.53134328358208949</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="54" t="s">
         <v>88</v>
       </c>
@@ -3310,7 +3230,7 @@
         <v>0.38507462686567184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>62</v>
       </c>
@@ -3336,7 +3256,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="54" t="s">
         <v>88</v>
       </c>
@@ -3356,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="54" t="s">
         <v>53</v>
       </c>
@@ -3379,7 +3299,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="54" t="s">
         <v>88</v>
       </c>
@@ -3399,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>61</v>
       </c>
@@ -3425,7 +3345,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="54" t="s">
         <v>88</v>
       </c>
@@ -3445,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="54" t="s">
         <v>53</v>
       </c>
@@ -3468,7 +3388,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="54" t="s">
         <v>88</v>
       </c>
@@ -3488,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>95</v>
       </c>
@@ -3514,7 +3434,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="54" t="s">
         <v>88</v>
       </c>
@@ -3535,7 +3455,7 @@
       </c>
       <c r="I14" s="27"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="54" t="s">
         <v>53</v>
       </c>
@@ -3559,7 +3479,7 @@
       </c>
       <c r="I15" s="27"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="54" t="s">
         <v>88</v>
       </c>
@@ -3580,7 +3500,7 @@
       </c>
       <c r="I16" s="27"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
         <v>76</v>
       </c>
@@ -3607,7 +3527,7 @@
       </c>
       <c r="I17" s="27"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" s="54" t="s">
         <v>84</v>
       </c>
@@ -3628,7 +3548,7 @@
       </c>
       <c r="I18" s="27"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
         <v>75</v>
       </c>
@@ -3654,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="54" t="s">
         <v>84</v>
       </c>
@@ -3674,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="54" t="s">
         <v>74</v>
       </c>
@@ -3700,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" s="54" t="s">
         <v>84</v>
       </c>
@@ -3720,7 +3640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="54" t="s">
         <v>94</v>
       </c>
@@ -3746,7 +3666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="54" t="s">
         <v>84</v>
       </c>
@@ -3766,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="54" t="s">
         <v>88</v>
       </c>
@@ -3786,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
         <v>93</v>
       </c>
@@ -3812,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="54" t="s">
         <v>84</v>
       </c>
@@ -3832,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="54" t="s">
         <v>88</v>
       </c>
@@ -3852,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
         <v>92</v>
       </c>
@@ -3878,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="54" t="s">
         <v>84</v>
       </c>
@@ -3898,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="54" t="s">
         <v>88</v>
       </c>
@@ -3918,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="54" t="s">
         <v>91</v>
       </c>
@@ -3944,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="54" t="s">
         <v>84</v>
       </c>
@@ -3964,7 +3884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="54" t="s">
         <v>88</v>
       </c>
@@ -3984,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="54" t="s">
         <v>90</v>
       </c>
@@ -4010,7 +3930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" s="54" t="s">
         <v>84</v>
       </c>
@@ -4030,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="54" t="s">
         <v>88</v>
       </c>
@@ -4050,7 +3970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="54" t="s">
         <v>89</v>
       </c>
@@ -4076,7 +3996,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="54" t="s">
         <v>84</v>
       </c>
@@ -4096,7 +4016,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="54" t="s">
         <v>88</v>
       </c>
@@ -4116,7 +4036,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="54" t="s">
         <v>40</v>
       </c>
@@ -4139,7 +4059,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="54" t="s">
         <v>84</v>
       </c>
@@ -4159,7 +4079,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="54" t="s">
         <v>88</v>
       </c>
@@ -4179,7 +4099,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="54" t="s">
         <v>87</v>
       </c>
@@ -4205,7 +4125,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="54" t="s">
         <v>84</v>
       </c>
@@ -4225,7 +4145,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="54" t="s">
         <v>86</v>
       </c>
@@ -4251,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="54" t="s">
         <v>84</v>
       </c>
@@ -4271,7 +4191,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="54" t="s">
         <v>154</v>
       </c>
@@ -4297,7 +4217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.15">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="54" t="s">
         <v>84</v>
       </c>
@@ -4324,26 +4244,26 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E47D49-C23B-C149-93F4-BADEC149BABD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.296875" style="1" customWidth="1"/>
     <col min="4" max="7" width="15.5" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
@@ -4365,7 +4285,7 @@
       </c>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>101</v>
       </c>
@@ -4389,7 +4309,7 @@
       </c>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>84</v>
       </c>
@@ -4407,7 +4327,7 @@
       </c>
       <c r="H3" s="37"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>100</v>
       </c>
@@ -4431,7 +4351,7 @@
       </c>
       <c r="H4" s="37"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
       <c r="C5" s="1" t="s">
         <v>84</v>
@@ -4450,7 +4370,7 @@
       </c>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>99</v>
       </c>
@@ -4474,7 +4394,7 @@
       </c>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="C7" s="1" t="s">
         <v>84</v>
@@ -4499,32 +4419,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CD15F7-5952-6543-B031-25026EC75539}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -4559,7 +4479,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>72</v>
       </c>
@@ -4576,7 +4496,7 @@
       <c r="J2" s="50"/>
       <c r="K2" s="50"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>101</v>
       </c>
@@ -4593,7 +4513,7 @@
       <c r="J3" s="50"/>
       <c r="K3" s="50"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
         <v>95</v>
       </c>
@@ -4610,7 +4530,7 @@
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>127</v>
       </c>
@@ -4627,7 +4547,7 @@
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>118</v>
       </c>
@@ -4646,7 +4566,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>75</v>
       </c>
@@ -4665,7 +4585,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>74</v>
       </c>
@@ -4684,7 +4604,7 @@
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>76</v>
       </c>
@@ -4703,7 +4623,7 @@
       <c r="J9" s="50"/>
       <c r="K9" s="50"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>149</v>
       </c>
@@ -4720,7 +4640,7 @@
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>150</v>
       </c>
@@ -4737,7 +4657,7 @@
       <c r="J11" s="50"/>
       <c r="K11" s="50"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>151</v>
       </c>
@@ -4754,7 +4674,7 @@
       <c r="J12" s="50"/>
       <c r="K12" s="50"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>152</v>
       </c>
@@ -4771,7 +4691,7 @@
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>148</v>
       </c>
@@ -4790,7 +4710,7 @@
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>153</v>
       </c>
@@ -4809,7 +4729,7 @@
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
         <v>70</v>
       </c>
@@ -4830,7 +4750,7 @@
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
         <v>77</v>
       </c>
@@ -4847,7 +4767,7 @@
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
         <v>114</v>
       </c>
@@ -4866,7 +4786,7 @@
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
         <v>113</v>
       </c>
@@ -4885,7 +4805,7 @@
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>112</v>
       </c>
@@ -4904,7 +4824,7 @@
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="54" t="s">
         <v>154</v>
       </c>
@@ -4923,7 +4843,7 @@
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="54" t="s">
         <v>61</v>
       </c>
@@ -4944,7 +4864,7 @@
       <c r="J22" s="50"/>
       <c r="K22" s="50"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="54" t="s">
         <v>69</v>
       </c>
@@ -4963,7 +4883,7 @@
       <c r="J23" s="50"/>
       <c r="K23" s="50"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="54" t="s">
         <v>99</v>
       </c>
@@ -4980,7 +4900,7 @@
       <c r="J24" s="50"/>
       <c r="K24" s="50"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
         <v>100</v>
       </c>
@@ -4997,7 +4917,7 @@
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
         <v>79</v>
       </c>
@@ -5014,7 +4934,7 @@
       <c r="J26" s="50"/>
       <c r="K26" s="50"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
         <v>71</v>
       </c>
@@ -5033,7 +4953,7 @@
       <c r="J27" s="50"/>
       <c r="K27" s="50"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
         <v>87</v>
       </c>
@@ -5050,7 +4970,7 @@
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
         <v>62</v>
       </c>
@@ -5069,7 +4989,7 @@
       <c r="J29" s="50"/>
       <c r="K29" s="50"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
         <v>82</v>
       </c>
@@ -5086,7 +5006,7 @@
       <c r="J30" s="50"/>
       <c r="K30" s="50"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
         <v>96</v>
       </c>
@@ -5105,7 +5025,7 @@
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="54" t="s">
         <v>90</v>
       </c>
@@ -5124,7 +5044,7 @@
       <c r="J32" s="50"/>
       <c r="K32" s="50"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
         <v>91</v>
       </c>
@@ -5143,7 +5063,7 @@
       <c r="J33" s="50"/>
       <c r="K33" s="50"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="54" t="s">
         <v>92</v>
       </c>
@@ -5162,7 +5082,7 @@
       <c r="J34" s="50"/>
       <c r="K34" s="50"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="54" t="s">
         <v>94</v>
       </c>
@@ -5181,7 +5101,7 @@
       <c r="J35" s="50"/>
       <c r="K35" s="50"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="54" t="s">
         <v>93</v>
       </c>
@@ -5200,7 +5120,7 @@
       <c r="J36" s="50"/>
       <c r="K36" s="50"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="54" t="s">
         <v>86</v>
       </c>
@@ -5217,7 +5137,7 @@
       <c r="J37" s="50"/>
       <c r="K37" s="50"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="54" t="s">
         <v>89</v>
       </c>
@@ -5247,7 +5167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CECF0B0-479E-404F-9D11-8B3773BD5FE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5257,22 +5177,22 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>126</v>
       </c>
@@ -5307,7 +5227,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -5336,7 +5256,7 @@
       <c r="J2" s="50"/>
       <c r="K2" s="50"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -5365,7 +5285,7 @@
       <c r="J3" s="50"/>
       <c r="K3" s="50"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -5394,7 +5314,7 @@
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -5423,7 +5343,7 @@
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -5452,7 +5372,7 @@
       <c r="J6" s="50"/>
       <c r="K6" s="50"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -5473,7 +5393,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -5494,7 +5414,7 @@
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -5515,7 +5435,7 @@
       <c r="J9" s="50"/>
       <c r="K9" s="50"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -5536,7 +5456,7 @@
       <c r="J10" s="50"/>
       <c r="K10" s="50"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -5557,7 +5477,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -5576,7 +5496,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -5595,7 +5515,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -5620,25 +5540,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CBF0B9-B848-6341-85A5-EAE471A5E15B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>109</v>
       </c>
@@ -5664,7 +5584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>133</v>
       </c>
@@ -5690,7 +5610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="57"/>
       <c r="C3" s="1" t="s">
         <v>104</v>
@@ -5712,7 +5632,7 @@
       </c>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="57"/>
       <c r="C4" s="1" t="s">
         <v>102</v>
@@ -5734,7 +5654,7 @@
       </c>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="57" t="s">
         <v>36</v>
       </c>
@@ -5758,7 +5678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="57"/>
       <c r="C6" s="1" t="s">
         <v>104</v>
@@ -5779,7 +5699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="57"/>
       <c r="C7" s="1" t="s">
         <v>102</v>
@@ -5800,7 +5720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="57" t="s">
         <v>35</v>
       </c>
@@ -5823,7 +5743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="57"/>
       <c r="C9" s="1" t="s">
         <v>104</v>
@@ -5844,7 +5764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="57"/>
       <c r="C10" s="1" t="s">
         <v>102</v>
@@ -5865,7 +5785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="57" t="s">
         <v>34</v>
       </c>
@@ -5888,7 +5808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="57"/>
       <c r="C12" s="1" t="s">
         <v>104</v>
@@ -5909,7 +5829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="57"/>
       <c r="C13" s="1" t="s">
         <v>102</v>
@@ -5930,7 +5850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="57" t="s">
         <v>33</v>
       </c>
@@ -5953,7 +5873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="57"/>
       <c r="C15" s="1" t="s">
         <v>104</v>
@@ -5974,7 +5894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="57"/>
       <c r="C16" s="1" t="s">
         <v>102</v>
@@ -5995,7 +5915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>103</v>
       </c>
@@ -6018,7 +5938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>135</v>
       </c>
@@ -6044,7 +5964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="57"/>
       <c r="C20" s="1" t="s">
         <v>104</v>
@@ -6065,7 +5985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="57"/>
       <c r="C21" s="1" t="s">
         <v>102</v>
@@ -6086,7 +6006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="57" t="s">
         <v>36</v>
       </c>
@@ -6109,7 +6029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="57"/>
       <c r="C23" s="1" t="s">
         <v>104</v>
@@ -6130,7 +6050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="57"/>
       <c r="C24" s="1" t="s">
         <v>102</v>
@@ -6151,7 +6071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="57" t="s">
         <v>35</v>
       </c>
@@ -6174,7 +6094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="57"/>
       <c r="C26" s="1" t="s">
         <v>104</v>
@@ -6195,7 +6115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="57"/>
       <c r="C27" s="1" t="s">
         <v>102</v>
@@ -6216,7 +6136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="57" t="s">
         <v>34</v>
       </c>
@@ -6239,7 +6159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="57"/>
       <c r="C29" s="1" t="s">
         <v>104</v>
@@ -6260,7 +6180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="57"/>
       <c r="C30" s="1" t="s">
         <v>102</v>
@@ -6281,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="57" t="s">
         <v>33</v>
       </c>
@@ -6304,7 +6224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="57"/>
       <c r="C32" s="1" t="s">
         <v>104</v>
@@ -6325,7 +6245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="57"/>
       <c r="C33" s="1" t="s">
         <v>102</v>
@@ -6346,7 +6266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="38" t="s">
         <v>103</v>
       </c>
@@ -6369,7 +6289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>134</v>
       </c>
@@ -6395,7 +6315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="57"/>
       <c r="C37" s="1" t="s">
         <v>104</v>
@@ -6416,7 +6336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="57"/>
       <c r="C38" s="1" t="s">
         <v>102</v>
@@ -6437,7 +6357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="57" t="s">
         <v>36</v>
       </c>
@@ -6460,7 +6380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="57"/>
       <c r="C40" s="1" t="s">
         <v>104</v>
@@ -6481,7 +6401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="57"/>
       <c r="C41" s="1" t="s">
         <v>102</v>
@@ -6502,7 +6422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="57" t="s">
         <v>35</v>
       </c>
@@ -6525,7 +6445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="57"/>
       <c r="C43" s="1" t="s">
         <v>104</v>
@@ -6546,7 +6466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="57"/>
       <c r="C44" s="1" t="s">
         <v>102</v>
@@ -6567,7 +6487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="57" t="s">
         <v>34</v>
       </c>
@@ -6590,7 +6510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="57"/>
       <c r="C46" s="1" t="s">
         <v>104</v>
@@ -6611,7 +6531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="57"/>
       <c r="C47" s="1" t="s">
         <v>102</v>
@@ -6632,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="57" t="s">
         <v>33</v>
       </c>
@@ -6655,7 +6575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="57"/>
       <c r="C49" s="1" t="s">
         <v>104</v>
@@ -6676,7 +6596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="57"/>
       <c r="C50" s="1" t="s">
         <v>102</v>
@@ -6697,7 +6617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="39" t="s">
         <v>103</v>
       </c>
@@ -6722,11 +6642,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -6737,6 +6652,11 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6744,7 +6664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A5AE56-D188-7745-8F54-E646EDECDF1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -6754,22 +6674,22 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" style="1" customWidth="1"/>
     <col min="5" max="6" width="13.5" style="1" customWidth="1"/>
     <col min="7" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24"/>
       <c r="C2" s="23" t="s">
         <v>22</v>
@@ -6784,7 +6704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>156</v>
       </c>
@@ -6794,7 +6714,7 @@
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>18</v>
       </c>
@@ -6811,7 +6731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>17</v>
       </c>
@@ -6828,7 +6748,7 @@
         <v>3.03</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
@@ -6845,7 +6765,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
@@ -6862,13 +6782,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="13"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -6886,14 +6806,14 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="13"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
@@ -6903,7 +6823,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -6913,7 +6833,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -6931,7 +6851,7 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -6949,7 +6869,7 @@
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -6967,7 +6887,7 @@
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="12"/>
@@ -6976,7 +6896,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -6987,7 +6907,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
@@ -7005,7 +6925,7 @@
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>6</v>
       </c>
@@ -7023,7 +6943,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
@@ -7041,7 +6961,7 @@
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
@@ -7059,7 +6979,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>3</v>
       </c>
@@ -7076,7 +6996,7 @@
         <v>999.99</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>2</v>
       </c>
@@ -7093,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>1</v>
       </c>
@@ -7110,7 +7030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>0</v>
       </c>
@@ -7127,10 +7047,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
   </sheetData>
@@ -7140,33 +7060,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A071D1F5-6005-5848-97E7-6A636059DF4C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
   <dimension ref="A1:P111"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.19921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
-    <col min="4" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="12" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="13.296875" style="1" customWidth="1"/>
+    <col min="9" max="12" width="13.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>125</v>
       </c>
@@ -7200,7 +7120,7 @@
       <c r="O2" s="28"/>
       <c r="P2" s="28"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>41</v>
@@ -7232,7 +7152,7 @@
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" s="26" t="s">
         <v>137</v>
       </c>
@@ -7260,7 +7180,7 @@
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5" s="26" t="s">
         <v>138</v>
       </c>
@@ -7288,7 +7208,7 @@
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C6" s="26" t="s">
         <v>139</v>
       </c>
@@ -7316,7 +7236,7 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
@@ -7347,7 +7267,7 @@
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" s="26" t="s">
         <v>137</v>
       </c>
@@ -7375,7 +7295,7 @@
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="26" t="s">
         <v>138</v>
       </c>
@@ -7403,7 +7323,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C10" s="26" t="s">
         <v>139</v>
       </c>
@@ -7431,7 +7351,7 @@
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
@@ -7462,7 +7382,7 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="26" t="s">
         <v>137</v>
       </c>
@@ -7490,7 +7410,7 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="26" t="s">
         <v>138</v>
       </c>
@@ -7518,7 +7438,7 @@
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14" s="26" t="s">
         <v>139</v>
       </c>
@@ -7546,7 +7466,7 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -7577,7 +7497,7 @@
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="26" t="s">
         <v>137</v>
       </c>
@@ -7605,7 +7525,7 @@
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C17" s="26" t="s">
         <v>138</v>
       </c>
@@ -7633,7 +7553,7 @@
       <c r="O17" s="25"/>
       <c r="P17" s="25"/>
     </row>
-    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="26" t="s">
         <v>139</v>
       </c>
@@ -7661,7 +7581,7 @@
       <c r="O18" s="25"/>
       <c r="P18" s="25"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="27" t="s">
         <v>39</v>
       </c>
@@ -7692,7 +7612,7 @@
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C20" s="26" t="s">
         <v>137</v>
       </c>
@@ -7720,7 +7640,7 @@
       <c r="O20" s="25"/>
       <c r="P20" s="25"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C21" s="26" t="s">
         <v>138</v>
       </c>
@@ -7748,7 +7668,7 @@
       <c r="O21" s="25"/>
       <c r="P21" s="25"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C22" s="26" t="s">
         <v>139</v>
       </c>
@@ -7776,7 +7696,7 @@
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>47</v>
       </c>
@@ -7807,7 +7727,7 @@
       <c r="O23" s="25"/>
       <c r="P23" s="25"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C24" s="26" t="s">
         <v>137</v>
       </c>
@@ -7835,7 +7755,7 @@
       <c r="O24" s="25"/>
       <c r="P24" s="25"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C25" s="26" t="s">
         <v>138</v>
       </c>
@@ -7863,7 +7783,7 @@
       <c r="O25" s="25"/>
       <c r="P25" s="25"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C26" s="26" t="s">
         <v>139</v>
       </c>
@@ -7891,12 +7811,12 @@
       <c r="O26" s="25"/>
       <c r="P26" s="25"/>
     </row>
-    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>130</v>
       </c>
@@ -7930,7 +7850,7 @@
       <c r="O29" s="28"/>
       <c r="P29" s="28"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>41</v>
@@ -7962,7 +7882,7 @@
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C31" s="26" t="s">
         <v>137</v>
       </c>
@@ -7990,7 +7910,7 @@
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C32" s="26" t="s">
         <v>53</v>
       </c>
@@ -8018,7 +7938,7 @@
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C33" s="26" t="s">
         <v>52</v>
       </c>
@@ -8046,7 +7966,7 @@
       <c r="O33" s="25"/>
       <c r="P33" s="25"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>40</v>
       </c>
@@ -8077,7 +7997,7 @@
       <c r="O34" s="25"/>
       <c r="P34" s="25"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C35" s="26" t="s">
         <v>137</v>
       </c>
@@ -8105,7 +8025,7 @@
       <c r="O35" s="25"/>
       <c r="P35" s="25"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C36" s="26" t="s">
         <v>53</v>
       </c>
@@ -8133,7 +8053,7 @@
       <c r="O36" s="25"/>
       <c r="P36" s="25"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C37" s="26" t="s">
         <v>52</v>
       </c>
@@ -8161,7 +8081,7 @@
       <c r="O37" s="25"/>
       <c r="P37" s="25"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
@@ -8192,7 +8112,7 @@
       <c r="O38" s="25"/>
       <c r="P38" s="25"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C39" s="26" t="s">
         <v>137</v>
       </c>
@@ -8220,7 +8140,7 @@
       <c r="O39" s="25"/>
       <c r="P39" s="25"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C40" s="26" t="s">
         <v>53</v>
       </c>
@@ -8248,7 +8168,7 @@
       <c r="O40" s="25"/>
       <c r="P40" s="25"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C41" s="26" t="s">
         <v>52</v>
       </c>
@@ -8276,7 +8196,7 @@
       <c r="O41" s="25"/>
       <c r="P41" s="25"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>48</v>
       </c>
@@ -8307,7 +8227,7 @@
       <c r="O42" s="25"/>
       <c r="P42" s="25"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C43" s="26" t="s">
         <v>137</v>
       </c>
@@ -8335,7 +8255,7 @@
       <c r="O43" s="25"/>
       <c r="P43" s="25"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C44" s="26" t="s">
         <v>53</v>
       </c>
@@ -8363,7 +8283,7 @@
       <c r="O44" s="25"/>
       <c r="P44" s="25"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C45" s="26" t="s">
         <v>52</v>
       </c>
@@ -8391,7 +8311,7 @@
       <c r="O45" s="25"/>
       <c r="P45" s="25"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>39</v>
       </c>
@@ -8422,7 +8342,7 @@
       <c r="O46" s="25"/>
       <c r="P46" s="25"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C47" s="26" t="s">
         <v>137</v>
       </c>
@@ -8450,7 +8370,7 @@
       <c r="O47" s="25"/>
       <c r="P47" s="25"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C48" s="26" t="s">
         <v>53</v>
       </c>
@@ -8478,7 +8398,7 @@
       <c r="O48" s="25"/>
       <c r="P48" s="25"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C49" s="26" t="s">
         <v>52</v>
       </c>
@@ -8506,7 +8426,7 @@
       <c r="O49" s="25"/>
       <c r="P49" s="25"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>47</v>
       </c>
@@ -8537,7 +8457,7 @@
       <c r="O50" s="25"/>
       <c r="P50" s="25"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C51" s="26" t="s">
         <v>137</v>
       </c>
@@ -8565,7 +8485,7 @@
       <c r="O51" s="25"/>
       <c r="P51" s="25"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C52" s="26" t="s">
         <v>53</v>
       </c>
@@ -8593,7 +8513,7 @@
       <c r="O52" s="25"/>
       <c r="P52" s="25"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C53" s="26" t="s">
         <v>52</v>
       </c>
@@ -8621,16 +8541,16 @@
       <c r="O53" s="25"/>
       <c r="P53" s="25"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
     </row>
-    <row r="55" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" s="27" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
         <v>124</v>
       </c>
@@ -8658,7 +8578,7 @@
       <c r="O56" s="28"/>
       <c r="P56" s="28"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>46</v>
@@ -8684,7 +8604,7 @@
       <c r="O57" s="25"/>
       <c r="P57" s="25"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C58" s="26" t="s">
         <v>141</v>
       </c>
@@ -8706,7 +8626,7 @@
       <c r="O58" s="25"/>
       <c r="P58" s="25"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>45</v>
       </c>
@@ -8731,7 +8651,7 @@
       <c r="O59" s="25"/>
       <c r="P59" s="25"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C60" s="26" t="s">
         <v>141</v>
       </c>
@@ -8753,7 +8673,7 @@
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>44</v>
       </c>
@@ -8778,7 +8698,7 @@
       <c r="O61" s="25"/>
       <c r="P61" s="25"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C62" s="26" t="s">
         <v>141</v>
       </c>
@@ -8800,16 +8720,16 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C63" s="26"/>
       <c r="D63" s="26"/>
     </row>
-    <row r="64" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" s="27" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
         <v>121</v>
       </c>
@@ -8843,7 +8763,7 @@
       <c r="O65" s="28"/>
       <c r="P65" s="28"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="51"/>
       <c r="B66" s="1" t="s">
         <v>7</v>
@@ -8875,7 +8795,7 @@
       <c r="O66" s="25"/>
       <c r="P66" s="25"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C67" s="26" t="s">
         <v>143</v>
       </c>
@@ -8903,7 +8823,7 @@
       <c r="O67" s="25"/>
       <c r="P67" s="25"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C68" s="26" t="s">
         <v>144</v>
       </c>
@@ -8931,7 +8851,7 @@
       <c r="O68" s="25"/>
       <c r="P68" s="25"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C69" s="26" t="s">
         <v>131</v>
       </c>
@@ -8959,7 +8879,7 @@
       <c r="O69" s="25"/>
       <c r="P69" s="25"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>6</v>
       </c>
@@ -8990,7 +8910,7 @@
       <c r="O70" s="25"/>
       <c r="P70" s="25"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C71" s="26" t="s">
         <v>143</v>
       </c>
@@ -9018,7 +8938,7 @@
       <c r="O71" s="25"/>
       <c r="P71" s="25"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C72" s="26" t="s">
         <v>144</v>
       </c>
@@ -9046,7 +8966,7 @@
       <c r="O72" s="25"/>
       <c r="P72" s="25"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C73" s="26" t="s">
         <v>131</v>
       </c>
@@ -9074,7 +8994,7 @@
       <c r="O73" s="25"/>
       <c r="P73" s="25"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>5</v>
       </c>
@@ -9105,7 +9025,7 @@
       <c r="O74" s="25"/>
       <c r="P74" s="25"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C75" s="26" t="s">
         <v>143</v>
       </c>
@@ -9133,7 +9053,7 @@
       <c r="O75" s="25"/>
       <c r="P75" s="25"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C76" s="26" t="s">
         <v>144</v>
       </c>
@@ -9161,7 +9081,7 @@
       <c r="O76" s="25"/>
       <c r="P76" s="25"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C77" s="26" t="s">
         <v>131</v>
       </c>
@@ -9189,7 +9109,7 @@
       <c r="O77" s="25"/>
       <c r="P77" s="25"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>3</v>
       </c>
@@ -9220,7 +9140,7 @@
       <c r="O78" s="25"/>
       <c r="P78" s="25"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C79" s="26" t="s">
         <v>143</v>
       </c>
@@ -9248,7 +9168,7 @@
       <c r="O79" s="25"/>
       <c r="P79" s="25"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C80" s="26" t="s">
         <v>144</v>
       </c>
@@ -9276,7 +9196,7 @@
       <c r="O80" s="25"/>
       <c r="P80" s="25"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C81" s="26" t="s">
         <v>131</v>
       </c>
@@ -9304,7 +9224,7 @@
       <c r="O81" s="25"/>
       <c r="P81" s="25"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>41</v>
       </c>
@@ -9335,7 +9255,7 @@
       <c r="O82" s="25"/>
       <c r="P82" s="25"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C83" s="26" t="s">
         <v>143</v>
       </c>
@@ -9363,7 +9283,7 @@
       <c r="O83" s="25"/>
       <c r="P83" s="25"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C84" s="26" t="s">
         <v>144</v>
       </c>
@@ -9391,7 +9311,7 @@
       <c r="O84" s="25"/>
       <c r="P84" s="25"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C85" s="26" t="s">
         <v>131</v>
       </c>
@@ -9419,7 +9339,7 @@
       <c r="O85" s="25"/>
       <c r="P85" s="25"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>40</v>
       </c>
@@ -9450,7 +9370,7 @@
       <c r="O86" s="25"/>
       <c r="P86" s="25"/>
     </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C87" s="26" t="s">
         <v>143</v>
       </c>
@@ -9478,7 +9398,7 @@
       <c r="O87" s="25"/>
       <c r="P87" s="25"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C88" s="26" t="s">
         <v>144</v>
       </c>
@@ -9506,7 +9426,7 @@
       <c r="O88" s="25"/>
       <c r="P88" s="25"/>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C89" s="26" t="s">
         <v>131</v>
       </c>
@@ -9534,7 +9454,7 @@
       <c r="O89" s="25"/>
       <c r="P89" s="25"/>
     </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>49</v>
       </c>
@@ -9565,7 +9485,7 @@
       <c r="O90" s="25"/>
       <c r="P90" s="25"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C91" s="26" t="s">
         <v>143</v>
       </c>
@@ -9593,7 +9513,7 @@
       <c r="O91" s="25"/>
       <c r="P91" s="25"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C92" s="26" t="s">
         <v>144</v>
       </c>
@@ -9621,7 +9541,7 @@
       <c r="O92" s="25"/>
       <c r="P92" s="25"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C93" s="26" t="s">
         <v>131</v>
       </c>
@@ -9649,7 +9569,7 @@
       <c r="O93" s="25"/>
       <c r="P93" s="25"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>39</v>
       </c>
@@ -9680,7 +9600,7 @@
       <c r="O94" s="25"/>
       <c r="P94" s="25"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C95" s="26" t="s">
         <v>143</v>
       </c>
@@ -9708,7 +9628,7 @@
       <c r="O95" s="25"/>
       <c r="P95" s="25"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C96" s="26" t="s">
         <v>144</v>
       </c>
@@ -9736,7 +9656,7 @@
       <c r="O96" s="25"/>
       <c r="P96" s="25"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C97" s="26" t="s">
         <v>131</v>
       </c>
@@ -9764,7 +9684,7 @@
       <c r="O97" s="25"/>
       <c r="P97" s="25"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>129</v>
       </c>
@@ -9795,7 +9715,7 @@
       <c r="O98" s="25"/>
       <c r="P98" s="25"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C99" s="26" t="s">
         <v>143</v>
       </c>
@@ -9823,7 +9743,7 @@
       <c r="O99" s="25"/>
       <c r="P99" s="25"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C100" s="26" t="s">
         <v>144</v>
       </c>
@@ -9851,7 +9771,7 @@
       <c r="O100" s="25"/>
       <c r="P100" s="25"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C101" s="26" t="s">
         <v>131</v>
       </c>
@@ -9879,12 +9799,12 @@
       <c r="O101" s="25"/>
       <c r="P101" s="25"/>
     </row>
-    <row r="103" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:16" s="27" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A104" s="31" t="s">
         <v>41</v>
       </c>
@@ -9918,7 +9838,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="27"/>
       <c r="C105" s="26" t="s">
@@ -9948,7 +9868,7 @@
       <c r="O105" s="25"/>
       <c r="P105" s="25"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C106" s="26" t="s">
         <v>143</v>
       </c>
@@ -9976,7 +9896,7 @@
       <c r="O106" s="25"/>
       <c r="P106" s="25"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C107" s="26" t="s">
         <v>144</v>
       </c>
@@ -10004,7 +9924,7 @@
       <c r="O107" s="25"/>
       <c r="P107" s="25"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C108" s="26" t="s">
         <v>131</v>
       </c>
@@ -10032,7 +9952,7 @@
       <c r="O108" s="25"/>
       <c r="P108" s="25"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
     </row>
   </sheetData>
@@ -10042,34 +9962,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B68D146-9822-8949-9710-2B0CED6E1AF5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.796875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>132</v>
       </c>
@@ -10090,7 +10010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
@@ -10110,7 +10030,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
         <v>128</v>
@@ -10131,12 +10051,12 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>62</v>
       </c>
@@ -10156,7 +10076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>61</v>
       </c>
@@ -10176,7 +10096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>89</v>
       </c>
@@ -10196,7 +10116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -10204,12 +10124,12 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
         <v>154</v>
@@ -10230,16 +10150,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>130</v>
       </c>
@@ -10262,7 +10182,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
         <v>58</v>
@@ -10283,7 +10203,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="51" t="s">
         <v>124</v>
       </c>
@@ -10291,28 +10211,28 @@
         <v>145</v>
       </c>
       <c r="C16" s="4">
-        <v>1.0249999999999999</v>
+        <v>1</v>
       </c>
       <c r="D16" s="4">
-        <v>1.0249999999999999</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4">
-        <v>1.0249999999999999</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4">
-        <v>1.0249999999999999</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4">
-        <v>1.0249999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" spans="1:6" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:6" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="43" t="s">
         <v>27</v>
       </c>
@@ -10326,7 +10246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>118</v>
       </c>
@@ -10351,7 +10271,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89648217-9EAE-DE4C-92EB-949BD9BE1394}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10361,7 +10281,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" style="1" customWidth="1"/>
     <col min="2" max="6" width="14.5" style="1"/>
@@ -10370,7 +10290,7 @@
     <col min="9" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
@@ -10388,7 +10308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>72</v>
       </c>
@@ -10408,7 +10328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="34" t="s">
         <v>67</v>
@@ -10426,7 +10346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>148</v>
       </c>
@@ -10446,7 +10366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="34" t="s">
         <v>67</v>
@@ -10464,7 +10384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>153</v>
       </c>
@@ -10484,7 +10404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="34" t="s">
         <v>67</v>
@@ -10502,7 +10422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>70</v>
       </c>
@@ -10522,7 +10442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="34" t="s">
         <v>67</v>
@@ -10540,7 +10460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>69</v>
       </c>
@@ -10560,7 +10480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="34" t="s">
         <v>67</v>
@@ -10578,7 +10498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>71</v>
       </c>
@@ -10598,7 +10518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
       <c r="B13" s="34" t="s">
         <v>67</v>
@@ -10616,10 +10536,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
     </row>
   </sheetData>
@@ -10629,7 +10549,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E60D92-0444-C14A-A043-D0BE8075CD64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10639,15 +10559,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="15" width="13.5" style="1" customWidth="1"/>
     <col min="16" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="22" t="s">
@@ -10690,12 +10610,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="35" t="s">
         <v>127</v>
       </c>
@@ -10739,7 +10659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
         <v>149</v>
       </c>
@@ -10783,7 +10703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="35" t="s">
         <v>150</v>
       </c>
@@ -10827,7 +10747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="35" t="s">
         <v>151</v>
       </c>
@@ -10871,7 +10791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="35" t="s">
         <v>152</v>
       </c>
@@ -10915,7 +10835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
         <v>148</v>
       </c>
@@ -10959,7 +10879,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="34" t="s">
         <v>153</v>
       </c>
@@ -11003,7 +10923,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="35" t="s">
         <v>70</v>
       </c>
@@ -11047,7 +10967,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>61</v>
       </c>
@@ -11091,7 +11011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="35" t="s">
         <v>69</v>
       </c>
@@ -11135,7 +11055,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="35" t="s">
         <v>79</v>
       </c>
@@ -11179,7 +11099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
         <v>71</v>
       </c>
@@ -11223,13 +11143,13 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="35"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="34" t="s">
         <v>75</v>
       </c>
@@ -11273,7 +11193,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="34" t="s">
         <v>74</v>
       </c>
@@ -11317,7 +11237,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
         <v>76</v>
       </c>
@@ -11361,7 +11281,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="34" t="s">
         <v>77</v>
       </c>
@@ -11405,16 +11325,16 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="26"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="26"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="26"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="26"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed default program names
</commit_message>
<xml_diff>
--- a/nutrition/default_params.xlsx
+++ b/nutrition/default_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/nutrition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B9B3420E-68BC-484E-BF03-B3E676AC1B9B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E48B666-71F4-E74A-9905-930C7C52D20A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <definedName name="stillbirth">'[1]Baseline year population inputs'!$C$27</definedName>
     <definedName name="term_SGA">'[1]Baseline year population inputs'!$C$35</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -625,18 +625,12 @@
     <t>IFAS (community)</t>
   </si>
   <si>
-    <t>IFAS (hospital)</t>
-  </si>
-  <si>
     <t>IFAS (retailer)</t>
   </si>
   <si>
     <t>IFAS (school)</t>
   </si>
   <si>
-    <t>IFAS for pregnant women (hospital)</t>
-  </si>
-  <si>
     <t>Kangaroo mother care</t>
   </si>
   <si>
@@ -653,6 +647,12 @@
   </si>
   <si>
     <t>Odds ratios for optimal birth spacing by program</t>
+  </si>
+  <si>
+    <t>IFAS for pregnant women (health facility)</t>
+  </si>
+  <si>
+    <t>IFAS (health facility)</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1251,9 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1538,7 +1540,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C7" s="50">
         <v>1</v>
@@ -2086,7 +2088,7 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="34" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C20" s="50">
         <v>0</v>
@@ -2415,7 +2417,7 @@
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43"/>
       <c r="B28" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C28" s="50">
         <v>0</v>
@@ -2459,7 +2461,7 @@
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C29" s="50">
         <v>0</v>
@@ -2503,7 +2505,7 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="50">
         <v>0</v>
@@ -4192,7 +4194,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48" s="54" t="s">
         <v>3</v>
@@ -4472,10 +4474,10 @@
         <v>119</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -4641,7 +4643,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
@@ -4658,7 +4660,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
@@ -4675,7 +4677,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
@@ -4711,7 +4713,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="34" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="50" t="s">
@@ -4825,7 +4827,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
@@ -5220,10 +5222,10 @@
         <v>119</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -6641,11 +6643,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -6656,6 +6653,11 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6705,7 +6707,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="21"/>
@@ -10125,13 +10127,13 @@
     </row>
     <row r="10" spans="1:7" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="4">
         <v>1.5</v>
@@ -10228,7 +10230,7 @@
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" spans="1:6" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -10385,7 +10387,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>68</v>
@@ -10704,7 +10706,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" s="35" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -10748,7 +10750,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B6" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -10792,7 +10794,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -10880,7 +10882,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B9" s="34" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>

</xml_diff>